<commit_message>
Initial commit of backend
</commit_message>
<xml_diff>
--- a/Project-Rubric.xlsx
+++ b/Project-Rubric.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Development/Udacity/Cloud/udacity-capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F80BA68-C6D3-5442-B69C-84E6ED608F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CE3DD6-DA20-5D46-846E-A3DCAF965D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22060" yWindow="9720" windowWidth="27640" windowHeight="16940" xr2:uid="{4C6129B8-E388-1A4C-9F5B-97A99D8C907E}"/>
+    <workbookView xWindow="22060" yWindow="9720" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{4C6129B8-E388-1A4C-9F5B-97A99D8C907E}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
+    <sheet name="Other" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Create Github repository with project code.</t>
   </si>
@@ -121,6 +122,15 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>CircleCI</t>
+  </si>
+  <si>
+    <t>https://app.circleci.com/pipelines/github/jpickup/udacity-capstone</t>
+  </si>
+  <si>
+    <t>GitHub</t>
   </si>
 </sst>
 </file>
@@ -511,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5E40D4E-87B5-F445-B980-06FC136D1127}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -641,4 +651,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CDDA89-C251-3746-89CE-26629B60BFA9}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>